<commit_message>
Comenzada función guardar_salir. Corregidas las funciones seleccionar_objetivo y sacar_lista. Hecha la función seleccionar_arma
</commit_message>
<xml_diff>
--- a/Armas_Hechizos.xlsx
+++ b/Armas_Hechizos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Python\PhytonMaster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB2A297-5E05-4226-86DE-1E90BEC7E02F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA7D32A-5D9E-40C6-96D2-8C24E3DE43EB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>1d8</t>
+  </si>
+  <si>
+    <t>Espada</t>
+  </si>
+  <si>
+    <t>3d4</t>
   </si>
 </sst>
 </file>
@@ -387,7 +393,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -428,6 +434,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" s="1"/>
     </row>

</xml_diff>